<commit_message>
Cố Gắng hoàn thành đúng thời gian để hoàn thiện review 1 và 2
</commit_message>
<xml_diff>
--- a/TastSheet/tasksheet.xlsx
+++ b/TastSheet/tasksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh-Shark\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eProject-WTW\TastSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -222,7 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +271,17 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -511,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -528,6 +539,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -537,6 +587,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -555,10 +635,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,71 +644,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,997 +946,1060 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="25.5">
-      <c r="A3" s="24" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="25">
+      <c r="A5" s="12">
         <v>1</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="25">
+      <c r="F5" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12">
         <v>3</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="25">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="25">
+      <c r="F6" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="12">
         <v>3</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="25">
+      <c r="A7" s="12">
         <v>3</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="25">
+      <c r="F7" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="12">
         <v>3</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="25">
+      <c r="A8" s="12">
         <v>4</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="25">
+      <c r="F8" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="12">
         <v>3</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="25">
+      <c r="A9" s="12">
         <v>5</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="25">
+      <c r="F9" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="12">
         <v>3</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="25">
+      <c r="A10" s="12">
         <v>6</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="25">
+      <c r="F10" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="12">
         <v>3</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="19"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="19">
+      <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19" t="s">
+      <c r="C13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="19"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="19">
+      <c r="A14" s="7">
         <v>8</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19" t="s">
+      <c r="C14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="19"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="19">
+      <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19" t="s">
+      <c r="C15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="19"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="19">
+      <c r="A16" s="7">
         <v>10</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19" t="s">
+      <c r="C16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="19"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="19">
+      <c r="A17" s="7">
         <v>11</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="C17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="19"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="19">
+      <c r="A18" s="7">
         <v>12</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19" t="s">
+      <c r="C18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="19">
+      <c r="A19" s="7">
         <v>13</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19" t="s">
+      <c r="C19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="19"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="19">
+      <c r="A20" s="7">
         <v>14</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
+      <c r="C20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="19"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="19">
+      <c r="A21" s="7">
         <v>15</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19" t="s">
+      <c r="C21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="19"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="19">
+      <c r="A22" s="7">
         <v>16</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="25" t="s">
+      <c r="C22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="F22" s="41">
+        <v>41548</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="19"/>
-      <c r="B23" s="32" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="19">
+      <c r="A24" s="7">
         <v>17</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19" t="s">
+      <c r="C24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="19">
+      <c r="A25" s="7">
         <v>18</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19" t="s">
+      <c r="C25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I25" s="19"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="19">
+      <c r="A26" s="7">
         <v>19</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
+      <c r="C26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="19"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="19">
+      <c r="A27" s="7">
         <v>20</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19" t="s">
+      <c r="C27" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="19"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="19">
+      <c r="A28" s="7">
         <v>21</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19" t="s">
+      <c r="C28" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I28" s="19"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="19">
+      <c r="A29" s="7">
         <v>22</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19" t="s">
+      <c r="C29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="19"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="19">
+      <c r="A30" s="7">
         <v>23</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19" t="s">
+      <c r="C30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="19"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="19">
+      <c r="A31" s="7">
         <v>24</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="25" t="s">
+      <c r="C31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19" t="s">
+      <c r="F31" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="19"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="19">
+      <c r="A32" s="7">
         <v>25</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19" t="s">
+      <c r="C32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="19"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="19"/>
-      <c r="B33" s="32" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="19">
+      <c r="A34" s="7">
         <v>26</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19" t="s">
+      <c r="C34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I34" s="19"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="19">
+      <c r="A35" s="7">
         <v>27</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
+      <c r="C35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="19"/>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="19">
+      <c r="A36" s="7">
         <v>28</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19" t="s">
+      <c r="C36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I36" s="19"/>
+      <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="19">
+      <c r="A37" s="7">
         <v>29</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19" t="s">
+      <c r="C37" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I37" s="19"/>
+      <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="19">
+      <c r="A38" s="7">
         <v>30</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19" t="s">
+      <c r="C38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="19"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="19">
-        <v>31</v>
-      </c>
-      <c r="B39" s="22" t="s">
+      <c r="A39" s="7">
+        <v>31</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19" t="s">
+      <c r="C39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I39" s="19"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="19"/>
-      <c r="B40" s="32" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="34"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="19">
+      <c r="A41" s="7">
         <v>32</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19" t="s">
+      <c r="C41" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="19"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="19">
+      <c r="A42" s="7">
         <v>33</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19" t="s">
+      <c r="C42" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I42" s="19"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="19">
-        <v>34</v>
-      </c>
-      <c r="B43" s="22" t="s">
+      <c r="A43" s="7">
+        <v>34</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19" t="s">
+      <c r="C43" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I43" s="19"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="19">
+      <c r="A44" s="7">
         <v>35</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19" t="s">
+      <c r="C44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I44" s="19"/>
+      <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="19">
+      <c r="A45" s="7">
         <v>36</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19" t="s">
+      <c r="C45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I45" s="19"/>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="19">
+      <c r="A46" s="7">
         <v>37</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+      <c r="C46" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="41">
+        <v>41548</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="25"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A48" s="16">
+      <c r="A48" s="6">
         <v>38</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
+      <c r="C48" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1">
       <c r="A49" s="1">
         <v>39</v>
       </c>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="3"/>
@@ -1930,13 +2010,13 @@
       <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A50" s="16">
+      <c r="A50" s="6">
         <v>40</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="3"/>
@@ -1950,10 +2030,10 @@
       <c r="A51" s="1">
         <v>41</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D51" s="3"/>
@@ -1964,13 +2044,13 @@
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A52" s="16">
+      <c r="A52" s="6">
         <v>42</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D52" s="3"/>
@@ -2146,15 +2226,15 @@
       <c r="I67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A68" s="6"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="8"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="21"/>
     </row>
     <row r="69" spans="1:9" ht="15.75" thickBot="1">
       <c r="A69" s="1"/>
@@ -2212,15 +2292,15 @@
       <c r="I73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A74" s="6"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="8"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="21"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" thickBot="1">
       <c r="A75" s="1"/>
@@ -2377,26 +2457,26 @@
       <c r="I88" s="3"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="9"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="9"/>
+      <c r="A89" s="32"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="36"/>
+      <c r="G89" s="32"/>
       <c r="H89" s="5"/>
-      <c r="I89" s="9"/>
+      <c r="I89" s="32"/>
     </row>
     <row r="90" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A90" s="10"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="10"/>
+      <c r="A90" s="33"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="33"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="10"/>
+      <c r="I90" s="33"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" thickBot="1">
       <c r="A91" s="1"/>
@@ -2707,15 +2787,15 @@
       <c r="I118" s="3"/>
     </row>
     <row r="119" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A119" s="6"/>
-      <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="I119" s="8"/>
+      <c r="A119" s="19"/>
+      <c r="B119" s="20"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+      <c r="I119" s="21"/>
     </row>
     <row r="120" spans="1:9" ht="15.75" thickBot="1">
       <c r="A120" s="1"/>
@@ -2762,15 +2842,15 @@
       <c r="I123" s="3"/>
     </row>
     <row r="124" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A124" s="6"/>
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="7"/>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-      <c r="G124" s="7"/>
-      <c r="H124" s="7"/>
-      <c r="I124" s="8"/>
+      <c r="A124" s="19"/>
+      <c r="B124" s="20"/>
+      <c r="C124" s="20"/>
+      <c r="D124" s="20"/>
+      <c r="E124" s="20"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="20"/>
+      <c r="H124" s="20"/>
+      <c r="I124" s="21"/>
     </row>
     <row r="125" spans="1:9" ht="15.75" thickBot="1">
       <c r="A125" s="1"/>
@@ -2795,15 +2875,15 @@
       <c r="I126" s="3"/>
     </row>
     <row r="127" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A127" s="6"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="7"/>
-      <c r="I127" s="8"/>
+      <c r="A127" s="19"/>
+      <c r="B127" s="20"/>
+      <c r="C127" s="20"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="20"/>
+      <c r="H127" s="20"/>
+      <c r="I127" s="21"/>
     </row>
     <row r="128" spans="1:9" ht="15.75" thickBot="1">
       <c r="A128" s="1"/>
@@ -2818,6 +2898,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A11:I11"/>
     <mergeCell ref="A119:I119"/>
     <mergeCell ref="A124:I124"/>
     <mergeCell ref="A127:I127"/>
@@ -2834,15 +2923,6 @@
     <mergeCell ref="C89:C90"/>
     <mergeCell ref="D89:D90"/>
     <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>